<commit_message>
update speed test results
</commit_message>
<xml_diff>
--- a/polyf3_benchmarks.xlsx
+++ b/polyf3_benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1D9A8B-1062-4566-848B-F851E5921AD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A045EE5-4F07-42BE-A889-A7D170DE368A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="12120" xr2:uid="{03C1E980-1D4C-40A8-AA63-4B8398A8299D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>hal_get_time</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -264,6 +264,26 @@
   </si>
   <si>
     <t>jump768divsteps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jump1521divsteps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mmul256x512s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>polyf3_mul768</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(subtract base value)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mmul768s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -628,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E647415-4C9E-4DBE-896E-04D2E38F3F27}">
-  <dimension ref="A2:F58"/>
+  <dimension ref="A2:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -866,7 +886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -881,7 +901,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -896,7 +916,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -911,7 +931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -926,7 +946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -941,12 +961,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -957,7 +980,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -969,7 +992,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -981,7 +1004,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -993,7 +1016,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1005,7 +1028,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1016,7 +1039,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1028,7 +1051,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1040,7 +1063,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1052,7 +1075,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1113,239 +1136,287 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C38">
-        <v>3774</v>
+        <v>129605</v>
       </c>
       <c r="F38">
-        <f>8*(C33-13)+4*(C24-13)</f>
-        <v>3836</v>
+        <f>9*(C36-13)+6*(C27-13)</f>
+        <v>126453</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39">
-        <v>12213</v>
+        <v>3980</v>
       </c>
       <c r="F39">
-        <f t="shared" ref="F39:F41" si="3">8*(C34-13)+4*(C25-13)</f>
-        <v>12272</v>
+        <f>8*(C33-13)+4*(C24-13)+205</f>
+        <v>4041</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C40">
-        <v>36866</v>
+        <v>12412</v>
       </c>
       <c r="F40">
-        <f t="shared" si="3"/>
-        <v>36920</v>
+        <f t="shared" ref="F40:F42" si="3">8*(C34-13)+4*(C25-13)+205</f>
+        <v>12477</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C41">
-        <v>111978</v>
+        <v>37075</v>
       </c>
       <c r="F41">
         <f t="shared" si="3"/>
-        <v>112040</v>
+        <v>37125</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C42">
-        <v>3614</v>
-      </c>
-      <c r="E42">
-        <f>(C38-C42)*100/C38</f>
-        <v>4.2395336512983572</v>
+        <v>112172</v>
       </c>
       <c r="F42">
-        <f>6*(C23-13)+4*(C28-13)+7*(C33-13)+6*(C24-13)+2*(C29-13)</f>
-        <v>3953</v>
+        <f t="shared" si="3"/>
+        <v>112245</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43">
-        <v>11561</v>
+        <v>3745</v>
       </c>
       <c r="E43">
-        <f t="shared" ref="E43:E45" si="4">(C39-C43)*100/C39</f>
-        <v>5.3385736510275938</v>
+        <f>(C39-C43)*100/C39</f>
+        <v>5.9045226130653266</v>
       </c>
       <c r="F43">
-        <f t="shared" ref="F43:F45" si="5">6*(C24-13)+4*(C29-13)+7*(C34-13)+6*(C25-13)+2*(C30-13)</f>
-        <v>11776</v>
+        <f>6*(C23-13)+4*(C28-13)+7*(C33-13)+6*(C24-13)+2*(C29-13)+205</f>
+        <v>4158</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44">
-        <v>34686</v>
+        <v>11642</v>
       </c>
       <c r="E44">
-        <f t="shared" si="4"/>
-        <v>5.9133076547496337</v>
+        <f t="shared" ref="E44:E46" si="4">(C40-C44)*100/C40</f>
+        <v>6.2036738640025781</v>
       </c>
       <c r="F44">
-        <f t="shared" si="5"/>
-        <v>33909</v>
+        <f t="shared" ref="F44:F47" si="5">6*(C24-13)+4*(C29-13)+7*(C34-13)+6*(C25-13)+2*(C30-13)+205</f>
+        <v>11981</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45">
-        <v>103320</v>
+        <v>34651</v>
       </c>
       <c r="E45">
         <f t="shared" si="4"/>
-        <v>7.7318759041954666</v>
+        <v>6.5380984490896834</v>
       </c>
       <c r="F45">
         <f t="shared" si="5"/>
-        <v>100837</v>
+        <v>34114</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C46">
-        <v>169</v>
+        <v>103824</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="4"/>
+        <v>7.4421424241343654</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="5"/>
+        <v>101042</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C47">
-        <v>2076</v>
+        <v>210693</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="5"/>
+        <v>209826</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="C48">
-        <v>6271</v>
+        <v>917703</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C49">
-        <v>18526</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C50">
-        <v>55960</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C51">
-        <v>2263</v>
+        <v>6271</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C52">
-        <v>18839</v>
-      </c>
-      <c r="F52">
-        <f>2*(C51-13)+(C42-13)</f>
-        <v>8101</v>
+        <v>18526</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C53">
-        <v>60028</v>
-      </c>
-      <c r="F53">
-        <f t="shared" ref="F53:F55" si="6">2*(C52-13)+(C43-13)</f>
-        <v>49200</v>
+        <v>55960</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C54">
-        <v>165462</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="6"/>
-        <v>154703</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C55">
-        <v>444997</v>
+        <v>23289</v>
       </c>
       <c r="F55">
-        <f t="shared" si="6"/>
-        <v>434205</v>
+        <f>2*(C54-13)+(C43-13)</f>
+        <v>12700</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="C56">
-        <v>839771</v>
+        <v>68929</v>
+      </c>
+      <c r="F56">
+        <f>2*(C55-13)+(C44-13)</f>
+        <v>58181</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>23</v>
-      </c>
-      <c r="B57">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C57">
-        <v>13</v>
+        <v>183262</v>
+      </c>
+      <c r="F57">
+        <f>2*(C56-13)+(C45-13)</f>
+        <v>172470</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58">
+        <v>480598</v>
+      </c>
+      <c r="F58">
+        <f>2*(C57-13)+(C46-13)</f>
+        <v>470309</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59">
+        <v>893073</v>
+      </c>
+      <c r="F59">
+        <f>(C58-13)+(C57-13)+(C47-13)</f>
+        <v>874514</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60">
+        <v>2045450</v>
+      </c>
+      <c r="F60">
+        <f>(C59-13)+(C58-13)+(C56-13)+(C55-13)+2*(C54-13)+(C39-13)+(C43-13)+(C44-13)+(C45-13)+(C47-13)+2*(C38-13)+2*205+2*(C5-13)</f>
+        <v>1999857</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61">
+        <v>41</v>
+      </c>
+      <c r="C61">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
         <v>24</v>
       </c>
-      <c r="B58">
+      <c r="B62">
         <v>42</v>
       </c>
-      <c r="C58">
+      <c r="C62">
         <v>14</v>
       </c>
     </row>

</xml_diff>